<commit_message>
Change name of constants worksheet
</commit_message>
<xml_diff>
--- a/storage/test_data/etl/d1_with_global_settings.xlsx
+++ b/storage/test_data/etl/d1_with_global_settings.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="sem" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="constants" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="mc constants" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -180,7 +180,7 @@
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -262,9 +262,9 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.96"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>